<commit_message>
add save and load model in c++ notebook
</commit_message>
<xml_diff>
--- a/C++_results.xlsx
+++ b/C++_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>classifier</t>
   </si>
@@ -31,6 +31,9 @@
     <t>classificationReport</t>
   </si>
   <si>
+    <t>AUC</t>
+  </si>
+  <si>
     <t>MCC</t>
   </si>
   <si>
@@ -58,60 +61,46 @@
     <t>lda</t>
   </si>
   <si>
-    <t>[[11  9]
- [ 0 58]]</t>
-  </si>
-  <si>
-    <t>[[15  5]
- [ 4 54]]</t>
-  </si>
-  <si>
-    <t>[[20  0]
- [ 6 52]]</t>
-  </si>
-  <si>
-    <t>[[19  1]
- [ 3 55]]</t>
-  </si>
-  <si>
-    <t>[[ 7 13]
- [ 0 58]]</t>
-  </si>
-  <si>
-    <t>[[15  5]
- [ 0 58]]</t>
-  </si>
-  <si>
-    <t>[[18  2]
- [ 1 57]]</t>
-  </si>
-  <si>
-    <t>[[ 0 20]
- [ 0 58]]</t>
-  </si>
-  <si>
-    <t>{'Flaky': {'precision': 1.0, 'recall': 0.55, 'f1-score': 0.7096774193548387, 'support': 20.0}, 'NonFlaky': {'precision': 0.8656716417910447, 'recall': 1.0, 'f1-score': 0.928, 'support': 58.0}, 'accuracy': 0.8846153846153846, 'macro avg': {'precision': 0.9328358208955223, 'recall': 0.775, 'f1-score': 0.8188387096774195, 'support': 78.0}, 'weighted avg': {'precision': 0.9001148105625717, 'recall': 0.8846153846153846, 'f1-score': 0.8720198511166254, 'support': 78.0}}</t>
-  </si>
-  <si>
-    <t>{'Flaky': {'precision': 0.7894736842105263, 'recall': 0.75, 'f1-score': 0.7692307692307692, 'support': 20.0}, 'NonFlaky': {'precision': 0.9152542372881356, 'recall': 0.9310344827586207, 'f1-score': 0.923076923076923, 'support': 58.0}, 'accuracy': 0.8846153846153846, 'macro avg': {'precision': 0.852363960749331, 'recall': 0.8405172413793103, 'f1-score': 0.846153846153846, 'support': 78.0}, 'weighted avg': {'precision': 0.8830028134220819, 'recall': 0.8846153846153846, 'f1-score': 0.883629191321499, 'support': 78.0}}</t>
-  </si>
-  <si>
-    <t>{'Flaky': {'precision': 0.7692307692307693, 'recall': 1.0, 'f1-score': 0.8695652173913044, 'support': 20.0}, 'NonFlaky': {'precision': 1.0, 'recall': 0.896551724137931, 'f1-score': 0.9454545454545454, 'support': 58.0}, 'accuracy': 0.9230769230769231, 'macro avg': {'precision': 0.8846153846153846, 'recall': 0.9482758620689655, 'f1-score': 0.907509881422925, 'support': 78.0}, 'weighted avg': {'precision': 0.9408284023668639, 'recall': 0.9230769230769231, 'f1-score': 0.9259957433870477, 'support': 78.0}}</t>
-  </si>
-  <si>
-    <t>{'Flaky': {'precision': 0.8636363636363636, 'recall': 0.95, 'f1-score': 0.9047619047619048, 'support': 20.0}, 'NonFlaky': {'precision': 0.9821428571428571, 'recall': 0.9482758620689655, 'f1-score': 0.9649122807017544, 'support': 58.0}, 'accuracy': 0.9487179487179487, 'macro avg': {'precision': 0.9228896103896104, 'recall': 0.9491379310344827, 'f1-score': 0.9348370927318296, 'support': 78.0}, 'weighted avg': {'precision': 0.9517565767565765, 'recall': 0.9487179487179487, 'f1-score': 0.9494891073838443, 'support': 78.0}}</t>
-  </si>
-  <si>
-    <t>{'Flaky': {'precision': 1.0, 'recall': 0.35, 'f1-score': 0.5185185185185185, 'support': 20.0}, 'NonFlaky': {'precision': 0.8169014084507042, 'recall': 1.0, 'f1-score': 0.8992248062015504, 'support': 58.0}, 'accuracy': 0.8333333333333334, 'macro avg': {'precision': 0.9084507042253521, 'recall': 0.675, 'f1-score': 0.7088716623600344, 'support': 78.0}, 'weighted avg': {'precision': 0.863849765258216, 'recall': 0.8333333333333334, 'f1-score': 0.8016078093597474, 'support': 78.0}}</t>
-  </si>
-  <si>
-    <t>{'Flaky': {'precision': 1.0, 'recall': 0.75, 'f1-score': 0.8571428571428571, 'support': 20.0}, 'NonFlaky': {'precision': 0.9206349206349206, 'recall': 1.0, 'f1-score': 0.9586776859504132, 'support': 58.0}, 'accuracy': 0.9358974358974359, 'macro avg': {'precision': 0.9603174603174602, 'recall': 0.875, 'f1-score': 0.9079102715466352, 'support': 78.0}, 'weighted avg': {'precision': 0.9409849409849409, 'recall': 0.9358974358974359, 'f1-score': 0.9326431144612963, 'support': 78.0}}</t>
-  </si>
-  <si>
-    <t>{'Flaky': {'precision': 0.9473684210526315, 'recall': 0.9, 'f1-score': 0.9230769230769231, 'support': 20.0}, 'NonFlaky': {'precision': 0.9661016949152542, 'recall': 0.9827586206896551, 'f1-score': 0.9743589743589743, 'support': 58.0}, 'accuracy': 0.9615384615384616, 'macro avg': {'precision': 0.9567350579839429, 'recall': 0.9413793103448276, 'f1-score': 0.9487179487179487, 'support': 78.0}, 'weighted avg': {'precision': 0.9612982913607356, 'recall': 0.9615384615384616, 'f1-score': 0.9612097304404997, 'support': 78.0}}</t>
-  </si>
-  <si>
-    <t>{'Flaky': {'precision': 0.0, 'recall': 0.0, 'f1-score': 0.0, 'support': 20.0}, 'NonFlaky': {'precision': 0.7435897435897436, 'recall': 1.0, 'f1-score': 0.8529411764705882, 'support': 58.0}, 'accuracy': 0.7435897435897436, 'macro avg': {'precision': 0.3717948717948718, 'recall': 0.5, 'f1-score': 0.4264705882352941, 'support': 78.0}, 'weighted avg': {'precision': 0.5529257067718607, 'recall': 0.7435897435897436, 'f1-score': 0.6342383107088989, 'support': 78.0}}</t>
+    <t>[[ 2  3]
+ [ 0 19]]</t>
+  </si>
+  <si>
+    <t>[[ 4  1]
+ [ 0 19]]</t>
+  </si>
+  <si>
+    <t>[[ 5  0]
+ [ 3 16]]</t>
+  </si>
+  <si>
+    <t>[[ 5  0]
+ [ 2 17]]</t>
+  </si>
+  <si>
+    <t>[[ 0  5]
+ [ 0 19]]</t>
+  </si>
+  <si>
+    <t>[[ 5  0]
+ [ 1 18]]</t>
+  </si>
+  <si>
+    <t>{'Flaky': {'precision': 1.0, 'recall': 0.4, 'f1-score': 0.5714285714285715, 'support': 5.0}, 'NonFlaky': {'precision': 0.8636363636363636, 'recall': 1.0, 'f1-score': 0.9268292682926829, 'support': 19.0}, 'accuracy': 0.875, 'macro avg': {'precision': 0.9318181818181819, 'recall': 0.7, 'f1-score': 0.7491289198606272, 'support': 24.0}, 'weighted avg': {'precision': 0.8920454545454546, 'recall': 0.875, 'f1-score': 0.8527874564459931, 'support': 24.0}}</t>
+  </si>
+  <si>
+    <t>{'Flaky': {'precision': 1.0, 'recall': 0.8, 'f1-score': 0.888888888888889, 'support': 5.0}, 'NonFlaky': {'precision': 0.95, 'recall': 1.0, 'f1-score': 0.9743589743589743, 'support': 19.0}, 'accuracy': 0.9583333333333334, 'macro avg': {'precision': 0.975, 'recall': 0.9, 'f1-score': 0.9316239316239316, 'support': 24.0}, 'weighted avg': {'precision': 0.9604166666666667, 'recall': 0.9583333333333334, 'f1-score': 0.9565527065527064, 'support': 24.0}}</t>
+  </si>
+  <si>
+    <t>{'Flaky': {'precision': 0.625, 'recall': 1.0, 'f1-score': 0.7692307692307693, 'support': 5.0}, 'NonFlaky': {'precision': 1.0, 'recall': 0.8421052631578947, 'f1-score': 0.9142857142857143, 'support': 19.0}, 'accuracy': 0.875, 'macro avg': {'precision': 0.8125, 'recall': 0.9210526315789473, 'f1-score': 0.8417582417582418, 'support': 24.0}, 'weighted avg': {'precision': 0.921875, 'recall': 0.875, 'f1-score': 0.884065934065934, 'support': 24.0}}</t>
+  </si>
+  <si>
+    <t>{'Flaky': {'precision': 0.7142857142857143, 'recall': 1.0, 'f1-score': 0.8333333333333333, 'support': 5.0}, 'NonFlaky': {'precision': 1.0, 'recall': 0.8947368421052632, 'f1-score': 0.9444444444444444, 'support': 19.0}, 'accuracy': 0.9166666666666666, 'macro avg': {'precision': 0.8571428571428572, 'recall': 0.9473684210526316, 'f1-score': 0.8888888888888888, 'support': 24.0}, 'weighted avg': {'precision': 0.9404761904761906, 'recall': 0.9166666666666666, 'f1-score': 0.9212962962962962, 'support': 24.0}}</t>
+  </si>
+  <si>
+    <t>{'Flaky': {'precision': 0.0, 'recall': 0.0, 'f1-score': 0.0, 'support': 5.0}, 'NonFlaky': {'precision': 0.7916666666666666, 'recall': 1.0, 'f1-score': 0.8837209302325582, 'support': 19.0}, 'accuracy': 0.7916666666666666, 'macro avg': {'precision': 0.3958333333333333, 'recall': 0.5, 'f1-score': 0.4418604651162791, 'support': 24.0}, 'weighted avg': {'precision': 0.626736111111111, 'recall': 0.7916666666666666, 'f1-score': 0.6996124031007752, 'support': 24.0}}</t>
+  </si>
+  <si>
+    <t>{'Flaky': {'precision': 0.8333333333333334, 'recall': 1.0, 'f1-score': 0.9090909090909091, 'support': 5.0}, 'NonFlaky': {'precision': 1.0, 'recall': 0.9473684210526315, 'f1-score': 0.972972972972973, 'support': 19.0}, 'accuracy': 0.9583333333333334, 'macro avg': {'precision': 0.9166666666666667, 'recall': 0.9736842105263157, 'f1-score': 0.941031941031941, 'support': 24.0}, 'weighted avg': {'precision': 0.9652777777777778, 'recall': 0.9583333333333334, 'f1-score': 0.9596642096642096, 'support': 24.0}}</t>
   </si>
 </sst>
 </file>
@@ -469,13 +458,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,188 +483,215 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2">
-        <v>0.8720198511166254</v>
+        <v>0.8527874564459931</v>
       </c>
       <c r="D2">
-        <v>0.8839285714285715</v>
+        <v>0.875</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G2">
-        <v>0.6900140599908632</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0.5877538136452587</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>0.883629191321499</v>
+        <v>0.9565527065527064</v>
       </c>
       <c r="D3">
-        <v>0.8732142857142857</v>
+        <v>0.9583333333333334</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G3">
-        <v>0.6927799185191492</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>0.9</v>
+      </c>
+      <c r="H3">
+        <v>0.8717797887081347</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4">
-        <v>0.9259957433870477</v>
+        <v>0.884065934065934</v>
       </c>
       <c r="D4">
-        <v>0.9232142857142858</v>
+        <v>0.875</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4">
-        <v>0.8304547985373997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>0.9210526315789473</v>
+      </c>
+      <c r="H4">
+        <v>0.7254762501100117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>0.9494891073838443</v>
+        <v>0.9212962962962962</v>
       </c>
       <c r="D5">
-        <v>0.9482142857142858</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G5">
-        <v>0.871632410288576</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0.7994358913389504</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6">
-        <v>0.8016078093597474</v>
+        <v>0.6996124031007752</v>
       </c>
       <c r="D6">
-        <v>0.8321428571428571</v>
+        <v>0.7916666666666666</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6">
-        <v>0.5347106628427626</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>0.5</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>0.9326431144612963</v>
+        <v>0.6996124031007752</v>
       </c>
       <c r="D7">
-        <v>0.9357142857142857</v>
+        <v>0.7916666666666666</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G7">
-        <v>0.8309489698388166</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8">
-        <v>0.9612097304404997</v>
+        <v>0.9596642096642096</v>
       </c>
       <c r="D8">
-        <v>0.9625</v>
+        <v>0.9583333333333334</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G8">
-        <v>0.8979830842577327</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0.8885233166386385</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9">
-        <v>0.6342383107088989</v>
+        <v>0.6996124031007752</v>
       </c>
       <c r="D9">
-        <v>0.7428571428571429</v>
+        <v>0.7916666666666666</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G9">
+        <v>0.8526315789473684</v>
+      </c>
+      <c r="H9">
         <v>0</v>
       </c>
     </row>

</xml_diff>